<commit_message>
Added functionality to Admin where it writes the collected Data to EmployeeInfo.csv and ValidLogins.csv, Added flag in Admin, Updated Contributions File
</commit_message>
<xml_diff>
--- a/CS4013ProjectTeamContributions.xlsx
+++ b/CS4013ProjectTeamContributions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iljablosenko/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctem1\OOP_ProjectV2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974F1A2-5BFC-1B4C-B446-B82491630E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56209AE7-8981-4AC1-B52E-71150D859B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="840" windowWidth="34200" windowHeight="21400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1815" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t xml:space="preserve">This contributions document must be agreed by all team members </t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Maksims</t>
+  </si>
+  <si>
+    <t>EmployeeInfo.csv</t>
+  </si>
+  <si>
+    <t>1 Hours</t>
+  </si>
+  <si>
+    <t>Ilja,Bri,Colin</t>
   </si>
 </sst>
 </file>
@@ -237,15 +246,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -565,40 +574,40 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="16.1640625" customWidth="1"/>
-    <col min="6" max="6" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="C2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -618,7 +627,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>23375493</v>
       </c>
@@ -638,7 +647,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23362901</v>
       </c>
@@ -658,7 +667,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>23363185</v>
       </c>
@@ -672,13 +681,13 @@
         <v>0.15</v>
       </c>
       <c r="E6" s="3">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="F6" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>23327936</v>
       </c>
@@ -692,13 +701,13 @@
         <v>0.2</v>
       </c>
       <c r="E7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="F7" s="3">
         <v>0.25</v>
       </c>
-      <c r="F7" s="3">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <f>SUM(C4:C7)</f>
         <v>1</v>
@@ -716,7 +725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
@@ -733,7 +742,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
@@ -750,7 +759,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -761,56 +770,74 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
+      <c r="B13">
+        <v>80</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
       <c r="F13" s="3">
-        <f t="shared" ref="F13:F21" si="1">SUM(B13:E13)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
+      <c r="C14">
+        <v>30</v>
+      </c>
+      <c r="D14">
+        <v>70</v>
+      </c>
       <c r="F14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>29</v>
       </c>
+      <c r="D15">
+        <v>100</v>
+      </c>
       <c r="F15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="C16">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>31</v>
       </c>
       <c r="C17">
-        <v>100</v>
+        <v>85</v>
+      </c>
+      <c r="D17">
+        <v>15</v>
       </c>
       <c r="F17" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -821,7 +848,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -832,7 +859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -843,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -854,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -871,59 +898,69 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23">
         <v>100</v>
       </c>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>100</v>
+      </c>
+      <c r="F24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F29" s="3"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F32" s="3"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="6" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>10</v>
       </c>
@@ -932,7 +969,7 @@
       <c r="D36" s="4"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>11</v>
       </c>
@@ -947,8 +984,8 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="7">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5">
         <v>45608</v>
       </c>
       <c r="C38" t="s">
@@ -959,8 +996,8 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="7">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
         <v>45611</v>
       </c>
       <c r="C39" t="s">
@@ -971,8 +1008,8 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="7">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
         <v>45616</v>
       </c>
       <c r="C40">
@@ -983,10 +1020,19 @@
       </c>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>45624</v>
+      </c>
+      <c r="C41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D41" t="s">
+        <v>43</v>
+      </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F42" s="3"/>
     </row>
   </sheetData>

</xml_diff>